<commit_message>
added experimental setup for gesturing
</commit_message>
<xml_diff>
--- a/Results/bodePlot23_09.xlsx
+++ b/Results/bodePlot23_09.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris.Chris-PC\Documents\robotLive\robot\robotTracking\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris.Chris-PC\Documents\robotLive\robot\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2853,11 +2853,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="248409176"/>
-        <c:axId val="248409568"/>
+        <c:axId val="230471776"/>
+        <c:axId val="230472168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="248409176"/>
+        <c:axId val="230471776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2914,12 +2914,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248409568"/>
+        <c:crossAx val="230472168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="248409568"/>
+        <c:axId val="230472168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2976,7 +2976,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248409176"/>
+        <c:crossAx val="230471776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3618,16 +3618,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>142142</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>508488</xdr:colOff>
       <xdr:row>1304</xdr:row>
-      <xdr:rowOff>47131</xdr:rowOff>
+      <xdr:rowOff>17823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>699370</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>208466</xdr:colOff>
       <xdr:row>1318</xdr:row>
-      <xdr:rowOff>123331</xdr:rowOff>
+      <xdr:rowOff>94023</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4204,8 +4204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1304" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1328" sqref="H1328"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>